<commit_message>
changes in login page test
</commit_message>
<xml_diff>
--- a/src/main/java/com/TestData/TorenzoTestData.xlsx
+++ b/src/main/java/com/TestData/TorenzoTestData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="645" windowWidth="18675" windowHeight="6660" activeTab="2"/>
+    <workbookView xWindow="720" yWindow="645" windowWidth="18675" windowHeight="6660"/>
   </bookViews>
   <sheets>
     <sheet name="LoginApp" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="67">
   <si>
     <t>Guest Name</t>
   </si>
@@ -215,6 +215,9 @@
   </si>
   <si>
     <t>Check whether navigated to home page upon clicking home button from payment page.</t>
+  </si>
+  <si>
+    <t>Check wheather Torenzocafe Title is displayed while clicking on "Cancel" from Role page.</t>
   </si>
 </sst>
 </file>
@@ -608,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,6 +773,14 @@
       </c>
       <c r="B17" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -834,7 +845,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
changes in after Class anotatio method
</commit_message>
<xml_diff>
--- a/src/main/java/com/TestData/TorenzoTestData.xlsx
+++ b/src/main/java/com/TestData/TorenzoTestData.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="68">
   <si>
     <t>Guest Name</t>
   </si>
@@ -218,6 +218,9 @@
   </si>
   <si>
     <t>Check wheather Torenzocafe Title is displayed while clicking on "Cancel" from Role page.</t>
+  </si>
+  <si>
+    <t>torenzocafe</t>
   </si>
 </sst>
 </file>
@@ -614,7 +617,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,7 +659,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
         <v>26</v>
@@ -767,7 +770,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -775,7 +778,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>66</v>
       </c>

</xml_diff>

<commit_message>
changes in class suspended page
</commit_message>
<xml_diff>
--- a/src/main/java/com/TestData/TorenzoTestData.xlsx
+++ b/src/main/java/com/TestData/TorenzoTestData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="645" windowWidth="18675" windowHeight="6660" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="720" yWindow="645" windowWidth="18675" windowHeight="6660" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="LoginApp" sheetId="2" r:id="rId1"/>
@@ -15,13 +15,14 @@
     <sheet name="ItemOperationPage" sheetId="7" r:id="rId6"/>
     <sheet name="TableStructure" sheetId="8" r:id="rId7"/>
     <sheet name="SuspendedOrder" sheetId="9" r:id="rId8"/>
+    <sheet name="OrderDiscount" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="220">
   <si>
     <t>Open Existing Restaurant/Store (Live Users)</t>
   </si>
@@ -630,14 +631,64 @@
   </si>
   <si>
     <t>Check whether we are navigated to table page from guest window.</t>
+  </si>
+  <si>
+    <t>Orders</t>
+  </si>
+  <si>
+    <t>To verify wheather Suspended Order list window Titile Is Displayed or not.</t>
+  </si>
+  <si>
+    <t>To verify Title of the Order page is displayed after clicking on "Cancel" button.</t>
+  </si>
+  <si>
+    <t>25365985</t>
+  </si>
+  <si>
+    <t>To verify the "Search Field" with invalid order number as input.</t>
+  </si>
+  <si>
+    <t>To verify wheather Search text got clear after upon clicking on Cancel button.</t>
+  </si>
+  <si>
+    <t>To verify wheather order list sort by cost in Decending order.</t>
+  </si>
+  <si>
+    <t>To verify wheather order list sort by cost in Ascending order.</t>
+  </si>
+  <si>
+    <t>Cost In Asc</t>
+  </si>
+  <si>
+    <t>Order No. in Dec</t>
+  </si>
+  <si>
+    <t>Cost In Dec</t>
+  </si>
+  <si>
+    <t>To verify wheather Order list sort by Order number in Decending Order.</t>
+  </si>
+  <si>
+    <t>To verify wheather Order list sort by Order number in Ascending Order.</t>
+  </si>
+  <si>
+    <t>Order No. in Asc</t>
+  </si>
+  <si>
+    <t>To verify Wheather order got searched from order list and selected successfully also it redirect to order page.</t>
+  </si>
+  <si>
+    <t>To verify wheather order data is reflected into orderEntry table or not.</t>
+  </si>
+  <si>
+    <t>Order With Item Names.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -692,7 +743,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -706,6 +757,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1016,9 +1076,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="46.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="64.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="1" max="1" width="46.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="64.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1195,9 +1255,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="49.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="45.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="1" max="1" width="49.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1248,9 +1308,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="41.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="83.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="1" max="1" width="41.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="83.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1400,9 +1460,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="81.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="81.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1450,8 +1510,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="42.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="86.0" collapsed="true"/>
+    <col min="1" max="1" width="42.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="86" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1634,8 +1694,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="31.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="109.42578125" collapsed="true"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="109.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2270,14 +2330,14 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D1" sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="32.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="76.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="1" max="1" width="32.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="76.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2320,6 +2380,9 @@
       <c r="B4" t="s">
         <v>193</v>
       </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -2327,6 +2390,9 @@
       </c>
       <c r="B5" t="s">
         <v>197</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2379,10 +2445,151 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.140625" style="7" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="95.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="B4" t="s">
+        <v>207</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="B5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B6" t="s">
+        <v>209</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="B7" t="s">
+        <v>210</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="B8" t="s">
+        <v>214</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="B9" t="s">
+        <v>215</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>217</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="B11" t="s">
+        <v>218</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
changes in User Details
</commit_message>
<xml_diff>
--- a/src/main/java/com/TestData/TorenzoTestData.xlsx
+++ b/src/main/java/com/TestData/TorenzoTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="645" windowWidth="18675" windowHeight="6660" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="720" yWindow="645" windowWidth="18675" windowHeight="6660" tabRatio="816" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="LoginApp" sheetId="2" r:id="rId1"/>
@@ -16,13 +16,14 @@
     <sheet name="TableStructure" sheetId="8" r:id="rId7"/>
     <sheet name="SuspendedOrder" sheetId="9" r:id="rId8"/>
     <sheet name="OrderDiscount" sheetId="10" r:id="rId9"/>
+    <sheet name="Sheet1" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="237">
   <si>
     <t>Open Existing Restaurant/Store (Live Users)</t>
   </si>
@@ -174,9 +175,6 @@
     <t>Check wheather Torenzocafe Title is displayed while clicking on "Cancel" from Role page.</t>
   </si>
   <si>
-    <t>torenzocafe</t>
-  </si>
-  <si>
     <t>User Details</t>
   </si>
   <si>
@@ -682,6 +680,60 @@
   </si>
   <si>
     <t>Order With Item Names.</t>
+  </si>
+  <si>
+    <t>Check wheather it is navigated on Reset Window and dispayed Torenzo café Title or not.</t>
+  </si>
+  <si>
+    <t>Torenzo Caf</t>
+  </si>
+  <si>
+    <t>Check with wheather invalid current pin Pin Got reset or not.</t>
+  </si>
+  <si>
+    <t>Pass New pin Number.</t>
+  </si>
+  <si>
+    <t>Pass New pin Number same as new pin.</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>12345678</t>
+  </si>
+  <si>
+    <t>Current Pin not matched.</t>
+  </si>
+  <si>
+    <t>Check Wheather Alert Massage is displyaed or not.</t>
+  </si>
+  <si>
+    <t>pass new pin Number</t>
+  </si>
+  <si>
+    <t>pass new pin To confirmed it .</t>
+  </si>
+  <si>
+    <t>pass valid current pin</t>
+  </si>
+  <si>
+    <t>Reset Password</t>
+  </si>
+  <si>
+    <t>Check wheather it is navigated on Reset Password Window and dispayed Torenzo café Title or not.</t>
+  </si>
+  <si>
+    <t>Check whether Alert message is displayed</t>
+  </si>
+  <si>
+    <t>Current Password not matched.</t>
+  </si>
+  <si>
+    <t>Your Password was successfully changed.</t>
+  </si>
+  <si>
+    <t>Check whether successfull Alert message is displyed.</t>
   </si>
 </sst>
 </file>
@@ -706,7 +758,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -731,6 +783,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -744,7 +802,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -767,6 +825,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1071,8 +1136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1114,7 +1179,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -1242,6 +1307,18 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1251,7 +1328,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1426,10 +1503,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C11" t="s">
         <v>25</v>
@@ -1437,10 +1514,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C12" t="s">
         <v>25</v>
@@ -1453,21 +1530,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" style="7" width="26.7109375" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="81.85546875" collapsed="true"/>
     <col min="3" max="3" customWidth="true" width="9.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -1478,22 +1555,155 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
         <v>51</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>52</v>
       </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>53</v>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="B4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="B5" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="B6" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="B7" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="B8" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
+      <c r="B13" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="C13" s="10"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="B14" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="B18" t="s">
+        <v>233</v>
+      </c>
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="B22" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1528,10 +1738,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
         <v>54</v>
-      </c>
-      <c r="B2" t="s">
-        <v>55</v>
       </c>
       <c r="C2" t="s">
         <v>25</v>
@@ -1539,10 +1749,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
         <v>56</v>
-      </c>
-      <c r="B3" t="s">
-        <v>57</v>
       </c>
       <c r="C3" t="s">
         <v>25</v>
@@ -1550,10 +1760,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" t="s">
         <v>58</v>
-      </c>
-      <c r="B4" t="s">
-        <v>59</v>
       </c>
       <c r="C4" t="s">
         <v>25</v>
@@ -1561,10 +1771,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" t="s">
         <v>60</v>
-      </c>
-      <c r="B5" t="s">
-        <v>61</v>
       </c>
       <c r="C5" t="s">
         <v>25</v>
@@ -1572,10 +1782,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
         <v>62</v>
-      </c>
-      <c r="B6" t="s">
-        <v>63</v>
       </c>
       <c r="C6" t="s">
         <v>25</v>
@@ -1583,10 +1793,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" t="s">
         <v>64</v>
-      </c>
-      <c r="B7" t="s">
-        <v>65</v>
       </c>
       <c r="C7" t="s">
         <v>25</v>
@@ -1594,10 +1804,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C8" t="s">
         <v>25</v>
@@ -1605,10 +1815,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" t="s">
         <v>68</v>
-      </c>
-      <c r="B9" t="s">
-        <v>69</v>
       </c>
       <c r="C9" t="s">
         <v>25</v>
@@ -1616,10 +1826,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
         <v>25</v>
@@ -1627,10 +1837,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" t="s">
         <v>72</v>
-      </c>
-      <c r="B11" t="s">
-        <v>73</v>
       </c>
       <c r="C11" t="s">
         <v>25</v>
@@ -1638,10 +1848,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" t="s">
         <v>74</v>
-      </c>
-      <c r="B12" t="s">
-        <v>75</v>
       </c>
       <c r="C12" t="s">
         <v>25</v>
@@ -1649,10 +1859,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C13" t="s">
         <v>25</v>
@@ -1660,10 +1870,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C14" t="s">
         <v>25</v>
@@ -1671,10 +1881,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" t="s">
         <v>78</v>
-      </c>
-      <c r="B15" t="s">
-        <v>79</v>
       </c>
       <c r="C15" t="s">
         <v>25</v>
@@ -1712,10 +1922,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" t="s">
         <v>81</v>
-      </c>
-      <c r="B2" t="s">
-        <v>82</v>
       </c>
       <c r="C2" t="s">
         <v>25</v>
@@ -1723,10 +1933,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C3" t="s">
         <v>25</v>
@@ -1734,10 +1944,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" t="s">
         <v>84</v>
-      </c>
-      <c r="B4" t="s">
-        <v>85</v>
       </c>
       <c r="C4" t="s">
         <v>25</v>
@@ -1745,10 +1955,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C5" t="s">
         <v>25</v>
@@ -1756,10 +1966,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" t="s">
         <v>88</v>
-      </c>
-      <c r="B6" t="s">
-        <v>89</v>
       </c>
       <c r="C6" t="s">
         <v>25</v>
@@ -1767,10 +1977,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" t="s">
         <v>94</v>
-      </c>
-      <c r="B7" t="s">
-        <v>95</v>
       </c>
       <c r="C7" t="s">
         <v>25</v>
@@ -1778,10 +1988,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" t="s">
         <v>96</v>
-      </c>
-      <c r="B8" t="s">
-        <v>97</v>
       </c>
       <c r="C8" t="s">
         <v>25</v>
@@ -1789,10 +1999,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B9" t="s">
         <v>98</v>
-      </c>
-      <c r="B9" t="s">
-        <v>99</v>
       </c>
       <c r="C9" t="s">
         <v>25</v>
@@ -1800,10 +2010,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" t="s">
         <v>100</v>
-      </c>
-      <c r="B10" t="s">
-        <v>101</v>
       </c>
       <c r="C10" t="s">
         <v>25</v>
@@ -1811,10 +2021,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" t="s">
         <v>102</v>
-      </c>
-      <c r="B11" t="s">
-        <v>103</v>
       </c>
       <c r="C11" t="s">
         <v>25</v>
@@ -1822,10 +2032,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12" t="s">
         <v>104</v>
-      </c>
-      <c r="B12" t="s">
-        <v>105</v>
       </c>
       <c r="C12" t="s">
         <v>25</v>
@@ -1833,10 +2043,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>105</v>
+      </c>
+      <c r="B13" t="s">
         <v>106</v>
-      </c>
-      <c r="B13" t="s">
-        <v>107</v>
       </c>
       <c r="C13" t="s">
         <v>25</v>
@@ -1844,10 +2054,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14" t="s">
         <v>108</v>
-      </c>
-      <c r="B14" t="s">
-        <v>109</v>
       </c>
       <c r="C14" t="s">
         <v>25</v>
@@ -1855,26 +2065,26 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" t="s">
         <v>110</v>
-      </c>
-      <c r="B15" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B16" t="s">
         <v>112</v>
-      </c>
-      <c r="B16" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>113</v>
+      </c>
+      <c r="B17" t="s">
         <v>114</v>
-      </c>
-      <c r="B17" t="s">
-        <v>115</v>
       </c>
       <c r="C17" t="s">
         <v>25</v>
@@ -1882,10 +2092,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C18" t="s">
         <v>25</v>
@@ -1893,10 +2103,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C19" t="s">
         <v>25</v>
@@ -1904,10 +2114,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>119</v>
+      </c>
+      <c r="B20" t="s">
         <v>120</v>
-      </c>
-      <c r="B20" t="s">
-        <v>121</v>
       </c>
       <c r="C20" t="s">
         <v>25</v>
@@ -1915,10 +2125,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>121</v>
+      </c>
+      <c r="B21" t="s">
         <v>122</v>
-      </c>
-      <c r="B21" t="s">
-        <v>123</v>
       </c>
       <c r="C21" t="s">
         <v>25</v>
@@ -1926,10 +2136,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>123</v>
+      </c>
+      <c r="B22" t="s">
         <v>124</v>
-      </c>
-      <c r="B22" t="s">
-        <v>125</v>
       </c>
       <c r="C22" t="s">
         <v>25</v>
@@ -1937,26 +2147,26 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B23" t="s">
         <v>126</v>
-      </c>
-      <c r="B23" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>127</v>
+      </c>
+      <c r="B24" t="s">
         <v>128</v>
-      </c>
-      <c r="B24" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C25" t="s">
         <v>25</v>
@@ -1964,10 +2174,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B26" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C26" t="s">
         <v>25</v>
@@ -1975,10 +2185,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C27" t="s">
         <v>25</v>
@@ -1986,10 +2196,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B28" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C28" t="s">
         <v>25</v>
@@ -1997,10 +2207,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B29" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C29" t="s">
         <v>25</v>
@@ -2008,10 +2218,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>134</v>
+      </c>
+      <c r="B30" t="s">
         <v>135</v>
-      </c>
-      <c r="B30" t="s">
-        <v>136</v>
       </c>
       <c r="C30" t="s">
         <v>25</v>
@@ -2019,10 +2229,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C31" t="s">
         <v>25</v>
@@ -2030,10 +2240,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B32" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C32" t="s">
         <v>25</v>
@@ -2041,10 +2251,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B33" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C33" t="s">
         <v>25</v>
@@ -2052,10 +2262,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C34" t="s">
         <v>25</v>
@@ -2063,10 +2273,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>144</v>
+      </c>
+      <c r="B35" t="s">
         <v>145</v>
-      </c>
-      <c r="B35" t="s">
-        <v>146</v>
       </c>
       <c r="C35" t="s">
         <v>25</v>
@@ -2074,10 +2284,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B36" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C36" t="s">
         <v>25</v>
@@ -2085,15 +2295,15 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>148</v>
+      </c>
+      <c r="B38" t="s">
         <v>149</v>
-      </c>
-      <c r="B38" t="s">
-        <v>150</v>
       </c>
       <c r="C38" t="s">
         <v>25</v>
@@ -2101,26 +2311,26 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B39" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B40" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B41" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C41" t="s">
         <v>25</v>
@@ -2128,10 +2338,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B42" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C42" t="s">
         <v>25</v>
@@ -2139,10 +2349,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B43" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C43" t="s">
         <v>25</v>
@@ -2150,10 +2360,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B44" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C44" t="s">
         <v>25</v>
@@ -2161,10 +2371,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>162</v>
+      </c>
+      <c r="B45" t="s">
         <v>163</v>
-      </c>
-      <c r="B45" t="s">
-        <v>164</v>
       </c>
       <c r="C45" t="s">
         <v>25</v>
@@ -2172,26 +2382,26 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B46" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B47" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B48" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C48" t="s">
         <v>25</v>
@@ -2199,10 +2409,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B49" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C49" t="s">
         <v>25</v>
@@ -2210,10 +2420,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B50" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C50" t="s">
         <v>25</v>
@@ -2221,29 +2431,29 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>174</v>
+      </c>
+      <c r="B51" t="s">
         <v>175</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
         <v>176</v>
-      </c>
-      <c r="C51" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B52" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>171</v>
+      </c>
+      <c r="B53" t="s">
         <v>172</v>
-      </c>
-      <c r="B53" t="s">
-        <v>173</v>
       </c>
       <c r="C53" t="s">
         <v>25</v>
@@ -2251,10 +2461,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B54" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C54" t="s">
         <v>25</v>
@@ -2262,18 +2472,18 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B55" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>180</v>
+      </c>
+      <c r="B56" t="s">
         <v>181</v>
-      </c>
-      <c r="B56" t="s">
-        <v>182</v>
       </c>
       <c r="C56" t="s">
         <v>25</v>
@@ -2281,10 +2491,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>182</v>
+      </c>
+      <c r="B57" t="s">
         <v>183</v>
-      </c>
-      <c r="B57" t="s">
-        <v>184</v>
       </c>
       <c r="C57" t="s">
         <v>25</v>
@@ -2292,18 +2502,18 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B58" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B59" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C59" t="s">
         <v>25</v>
@@ -2311,10 +2521,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B60" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C60" t="s">
         <v>25</v>
@@ -2354,10 +2564,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" t="s">
         <v>188</v>
-      </c>
-      <c r="B2" t="s">
-        <v>189</v>
       </c>
       <c r="C2" t="s">
         <v>25</v>
@@ -2365,10 +2575,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B3" t="s">
         <v>190</v>
-      </c>
-      <c r="B3" t="s">
-        <v>191</v>
       </c>
       <c r="C3" t="s">
         <v>25</v>
@@ -2376,10 +2586,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B4" t="s">
         <v>192</v>
-      </c>
-      <c r="B4" t="s">
-        <v>193</v>
       </c>
       <c r="C4" t="s">
         <v>25</v>
@@ -2387,10 +2597,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>195</v>
+      </c>
+      <c r="B5" t="s">
         <v>196</v>
-      </c>
-      <c r="B5" t="s">
-        <v>197</v>
       </c>
       <c r="C5" t="s">
         <v>25</v>
@@ -2398,10 +2608,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>193</v>
+      </c>
+      <c r="B6" t="s">
         <v>194</v>
-      </c>
-      <c r="B6" t="s">
-        <v>195</v>
       </c>
       <c r="C6" t="s">
         <v>25</v>
@@ -2409,18 +2619,18 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>198</v>
+      </c>
+      <c r="B7" t="s">
         <v>199</v>
-      </c>
-      <c r="B7" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C8" t="s">
         <v>25</v>
@@ -2428,10 +2638,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C9" t="s">
         <v>25</v>
@@ -2439,10 +2649,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>200</v>
+      </c>
+      <c r="B10" t="s">
         <v>201</v>
-      </c>
-      <c r="B10" t="s">
-        <v>202</v>
       </c>
       <c r="C10" t="s">
         <v>25</v>
@@ -2457,7 +2667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -2481,10 +2691,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="B2" t="s">
         <v>203</v>
-      </c>
-      <c r="B2" t="s">
-        <v>204</v>
       </c>
       <c r="C2" t="s">
         <v>25</v>
@@ -2495,7 +2705,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C3" t="s">
         <v>25</v>
@@ -2503,10 +2713,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="B4" t="s">
         <v>206</v>
-      </c>
-      <c r="B4" t="s">
-        <v>207</v>
       </c>
       <c r="C4" t="s">
         <v>25</v>
@@ -2514,10 +2724,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C5" t="s">
         <v>25</v>
@@ -2525,10 +2735,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C6" t="s">
         <v>25</v>
@@ -2536,10 +2746,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C7" t="s">
         <v>25</v>
@@ -2547,10 +2757,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C8" t="s">
         <v>25</v>
@@ -2558,10 +2768,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C9" t="s">
         <v>25</v>
@@ -2572,7 +2782,7 @@
         <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C10" t="s">
         <v>25</v>
@@ -2580,10 +2790,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C11" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Changes in multiple classes
</commit_message>
<xml_diff>
--- a/src/main/java/com/TestData/TorenzoTestData.xlsx
+++ b/src/main/java/com/TestData/TorenzoTestData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="645" windowWidth="18675" windowHeight="6660" tabRatio="816" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="720" yWindow="645" windowWidth="18675" windowHeight="6660" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="LoginApp" sheetId="2" r:id="rId1"/>
@@ -16,14 +16,16 @@
     <sheet name="TableStructure" sheetId="8" r:id="rId7"/>
     <sheet name="SuspendedOrder" sheetId="9" r:id="rId8"/>
     <sheet name="OrderDiscount" sheetId="10" r:id="rId9"/>
-    <sheet name="Sheet1" sheetId="11" r:id="rId10"/>
+    <sheet name="AdminSettingPage" sheetId="11" r:id="rId10"/>
+    <sheet name="EditOrderPage" sheetId="12" r:id="rId11"/>
+    <sheet name="User" sheetId="13" r:id="rId12"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="264">
   <si>
     <t>Open Existing Restaurant/Store (Live Users)</t>
   </si>
@@ -682,12 +684,99 @@
     <t>Order With Item Names.</t>
   </si>
   <si>
+    <t>Apply Discount</t>
+  </si>
+  <si>
+    <t>Verify Discount window is displayed upon clicking on disocunt</t>
+  </si>
+  <si>
+    <t>Verify order total on discount window</t>
+  </si>
+  <si>
+    <t>Verify order total is matched on discount window</t>
+  </si>
+  <si>
+    <t>Verify Order total is updated</t>
+  </si>
+  <si>
+    <t>Verify order total is update after giving order disocunt in percentage.</t>
+  </si>
+  <si>
+    <t>Verify order total is updated after removing the discount.</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Pass the discount amount and verify total</t>
+  </si>
+  <si>
+    <t>Verify order total is updated after removing the amount discount.</t>
+  </si>
+  <si>
+    <t>Verify Disocunt window is opened</t>
+  </si>
+  <si>
+    <t>Verify Disocunt window is opened after removing and adding new .</t>
+  </si>
+  <si>
+    <t>Check whether confirmation popup is displayed upon clicking on delete order amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check whether items are loaded from Admin Setting </t>
+  </si>
+  <si>
+    <t>Verify Item images displayed</t>
+  </si>
+  <si>
+    <t>Check whether items are displayed when checked from Admin Settings</t>
+  </si>
+  <si>
+    <t>Check whether tables are loaded when loaded from Admin Settings.</t>
+  </si>
+  <si>
+    <t>Verify Tables are loaded</t>
+  </si>
+  <si>
+    <t>Verify Items are loaded</t>
+  </si>
+  <si>
+    <t>Check whether Edit order window is displayed.</t>
+  </si>
+  <si>
+    <t>Verify date</t>
+  </si>
+  <si>
+    <t>Check whether date is matched with system date.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify We navigated </t>
+  </si>
+  <si>
+    <t>Check whether we navigated to home page aftre reloading home page.</t>
+  </si>
+  <si>
+    <t>Verify Order number</t>
+  </si>
+  <si>
+    <t>Check whether order number is matched after reloading edit order</t>
+  </si>
+  <si>
+    <t>Check whether order total is matched after reloading edit order</t>
+  </si>
+  <si>
+    <t>NCKOT</t>
+  </si>
+  <si>
+    <t>Check whether NCKOT order window is displayed.</t>
+  </si>
+  <si>
+    <t>Torenzo Caf</t>
+  </si>
+  <si>
     <t>Check wheather it is navigated on Reset Window and dispayed Torenzo café Title or not.</t>
   </si>
   <si>
-    <t>Torenzo Caf</t>
-  </si>
-  <si>
     <t>Check with wheather invalid current pin Pin Got reset or not.</t>
   </si>
   <si>
@@ -697,37 +786,31 @@
     <t>Pass New pin Number same as new pin.</t>
   </si>
   <si>
-    <t>123456</t>
-  </si>
-  <si>
-    <t>12345678</t>
-  </si>
-  <si>
     <t>Current Pin not matched.</t>
   </si>
   <si>
     <t>Check Wheather Alert Massage is displyaed or not.</t>
   </si>
   <si>
+    <t>pass valid current pin</t>
+  </si>
+  <si>
     <t>pass new pin Number</t>
   </si>
   <si>
     <t>pass new pin To confirmed it .</t>
   </si>
   <si>
-    <t>pass valid current pin</t>
-  </si>
-  <si>
     <t>Reset Password</t>
   </si>
   <si>
     <t>Check wheather it is navigated on Reset Password Window and dispayed Torenzo café Title or not.</t>
   </si>
   <si>
+    <t>Current Password not matched.</t>
+  </si>
+  <si>
     <t>Check whether Alert message is displayed</t>
-  </si>
-  <si>
-    <t>Current Password not matched.</t>
   </si>
   <si>
     <t>Your Password was successfully changed.</t>
@@ -740,8 +823,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -785,7 +867,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2"/>
+        <fgColor theme="3" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -802,7 +884,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -826,12 +908,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1136,15 +1215,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="46.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="64.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="1" max="1" width="46.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="64.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1312,6 +1391,214 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="66.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="B2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>233</v>
+      </c>
+      <c r="B3" t="s">
+        <v>234</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>236</v>
+      </c>
+      <c r="B4" t="s">
+        <v>235</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="66.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="B2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>241</v>
+      </c>
+      <c r="B4" t="s">
+        <v>242</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>243</v>
+      </c>
+      <c r="B5" t="s">
+        <v>244</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>198</v>
+      </c>
+      <c r="B6" t="s">
+        <v>245</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="10" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="B9" t="s">
+        <v>247</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>239</v>
+      </c>
+      <c r="B10" t="s">
+        <v>240</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>241</v>
+      </c>
+      <c r="B11" t="s">
+        <v>242</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>243</v>
+      </c>
+      <c r="B12" t="s">
+        <v>244</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>198</v>
+      </c>
+      <c r="B13" t="s">
+        <v>245</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1328,14 +1615,14 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="49.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="45.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="1" max="1" width="49.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1378,17 +1665,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="41.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="83.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="1" max="1" width="41.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="83.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1521,6 +1808,14 @@
       </c>
       <c r="C12" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" t="s">
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -1532,19 +1827,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="7" width="26.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="81.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="91.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -1555,7 +1850,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" t="s">
         <v>50</v>
       </c>
       <c r="B2" t="s">
@@ -1563,7 +1858,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
@@ -1571,135 +1866,133 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>220</v>
+      <c r="A4" t="s">
+        <v>248</v>
       </c>
       <c r="B4" t="s">
-        <v>219</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>224</v>
+      <c r="A5">
+        <v>123456</v>
       </c>
       <c r="B5" t="s">
-        <v>221</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>225</v>
+      <c r="A6">
+        <v>12345678</v>
       </c>
       <c r="B6" t="s">
-        <v>222</v>
+        <v>251</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>225</v>
+      <c r="A7">
+        <v>12345678</v>
       </c>
       <c r="B7" t="s">
-        <v>223</v>
+        <v>252</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>226</v>
+      <c r="A8" t="s">
+        <v>253</v>
       </c>
       <c r="B8" t="s">
-        <v>227</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>8</v>
+      <c r="A9">
+        <v>1234</v>
       </c>
       <c r="B9" t="s">
-        <v>230</v>
+        <v>255</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>8</v>
+      <c r="A10">
+        <v>1234</v>
       </c>
       <c r="B10" t="s">
-        <v>228</v>
+        <v>256</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>8</v>
+      <c r="A11">
+        <v>1234</v>
       </c>
       <c r="B11" t="s">
-        <v>229</v>
+        <v>257</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="C13" s="10"/>
+      <c r="B13" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>220</v>
+      <c r="A14" t="s">
+        <v>248</v>
       </c>
       <c r="B14" t="s">
-        <v>232</v>
+        <v>259</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>225</v>
+      <c r="A15">
+        <v>12345678</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>234</v>
+      <c r="A16">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>260</v>
       </c>
       <c r="B18" t="s">
-        <v>233</v>
+        <v>261</v>
       </c>
       <c r="C18" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
-        <v>235</v>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>262</v>
       </c>
       <c r="B22" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>28</v>
       </c>
       <c r="B23" t="s">
@@ -1716,13 +2009,13 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="42.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="86.0" collapsed="true"/>
+    <col min="1" max="1" width="42.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="86" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1900,13 +2193,13 @@
   <dimension ref="A1:C60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD4"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="31.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="109.42578125" collapsed="true"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="109.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2546,9 +2839,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="32.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="76.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="1" max="1" width="32.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="76.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2667,15 +2960,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection sqref="A1:R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="7" width="31.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="95.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="1" max="1" width="31.140625" style="7" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="95.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2806,14 +3099,108 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="36.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="74.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="B2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="B3" t="s">
+        <v>222</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="B4" t="s">
+        <v>224</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>223</v>
+      </c>
+      <c r="B5" t="s">
+        <v>225</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="B6" t="s">
+        <v>227</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>223</v>
+      </c>
+      <c r="B7" t="s">
+        <v>228</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>229</v>
+      </c>
+      <c r="B8" t="s">
+        <v>230</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>